<commit_message>
TC for Login added
</commit_message>
<xml_diff>
--- a/Test-Cases.xlsx
+++ b/Test-Cases.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b69f171f4aec32e/Documents/GithubProjects/Manual-Testing-E-commerce-Amazon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="542" documentId="8_{815BE7B0-3C72-4824-8212-FAF9C84139DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1076229F-10BB-48CA-A258-21C9E57D3DDE}"/>
+  <xr:revisionPtr revIDLastSave="673" documentId="8_{815BE7B0-3C72-4824-8212-FAF9C84139DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E39B122F-25F8-4306-9A41-93E79285B0F0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{6E1B6E8A-1244-4A63-966D-B4892D0CED0D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{6E1B6E8A-1244-4A63-966D-B4892D0CED0D}"/>
   </bookViews>
   <sheets>
     <sheet name="URL_Test_Cases" sheetId="1" r:id="rId1"/>
     <sheet name="User Registration_TestCases" sheetId="2" r:id="rId2"/>
-    <sheet name="Login_TestCases" sheetId="3" r:id="rId3"/>
+    <sheet name="Login&amp;Logout_TestCases" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="240">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -692,16 +693,146 @@
 3.click login</t>
   </si>
   <si>
-    <t>1.Enter Email.
-2.Enter Password</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.Enter Email.
 2.Enter Password
 3.Clik login </t>
   </si>
   <si>
     <t>Home Page to be displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Enter Email.
+2.Click on forgot Password
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reset Password page to  be-redirected </t>
+  </si>
+  <si>
+    <t>Valid email, password</t>
+  </si>
+  <si>
+    <t>Email ,password</t>
+  </si>
+  <si>
+    <t>Blank data</t>
+  </si>
+  <si>
+    <t>User should be able login to website successfully</t>
+  </si>
+  <si>
+    <t>Login Successful</t>
+  </si>
+  <si>
+    <t>1.Open the browser
+2.Ensure the user is logged out (or open a new incognito/private window)
+3.Directly enter a protected page URL in the address bar
+Press Enter</t>
+  </si>
+  <si>
+    <t>User should be redirected to the login page</t>
+  </si>
+  <si>
+    <t>Proctected URL</t>
+  </si>
+  <si>
+    <t>User is logged in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1.Open the application
+2.Ensure the user is logged in
+3.Click on Profile / Account / Logout option
+4.Confirm logout (if confirmation popup is shown)
+5.Observe the system behavior
+</t>
+  </si>
+  <si>
+    <t>User should be logged out successfully and
+ redirected to the login page or home page</t>
+  </si>
+  <si>
+    <t>1Open the application
+2.Ensure the user is logged in
+3.Click on Profile / Account / Logout option
+4.Confirm logout (if confirmation popup is shown)
+5.Observe the system behavior</t>
+  </si>
+  <si>
+    <t>1. Login to application
+2. Do not perform any activity
+3. Wait for configured session timeout duration</t>
+  </si>
+  <si>
+    <t>Idle time = configured timeout</t>
+  </si>
+  <si>
+    <t>User should be logged out automatically 
+and redirected to login page |</t>
+  </si>
+  <si>
+    <t>"Invalid credentials" or
+ "Incorrect email/password"</t>
+  </si>
+  <si>
+    <t>Error messages "Email is required" and
+ "Password is required" are displayed.</t>
+  </si>
+  <si>
+    <t>Invalid Email/Password
+ displayed on UI</t>
+  </si>
+  <si>
+    <t>Email and Password
+Required</t>
+  </si>
+  <si>
+    <t>"Invalid credentials" or
+ "password incorrect "</t>
+  </si>
+  <si>
+    <t>"Invalid credentials" or "password incorrect " message displayed when clicked on Login</t>
+  </si>
+  <si>
+    <t>"Email and Password required "</t>
+  </si>
+  <si>
+    <t>"Email and Password required "diplayed when clicked on login</t>
+  </si>
+  <si>
+    <t>"Password should be masked and clicked on eye should show the password"</t>
+  </si>
+  <si>
+    <t>1.Enter Email.
+2.Enter Password
+3.Clik outside</t>
+  </si>
+  <si>
+    <t>"Password is  masked and clicked on eye password is  showen"</t>
+  </si>
+  <si>
+    <t>"Re-directed to password reset page "</t>
+  </si>
+  <si>
+    <t>" Re-directed to Reset password  page"</t>
+  </si>
+  <si>
+    <t>"Login page redirected "</t>
+  </si>
+  <si>
+    <t>User is  not logged IN</t>
+  </si>
+  <si>
+    <t>"user logged out and directed to login page"</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Account created successfully </t>
+  </si>
+  <si>
+    <t>Phone number should be valid</t>
   </si>
 </sst>
 </file>
@@ -772,7 +903,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -810,7 +941,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -839,8 +969,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -857,6 +997,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1178,8 +1322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCD6D3BF-43B2-46AE-8869-8724C02B6152}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,7 +1416,9 @@
       <c r="K2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>237</v>
+      </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
@@ -1310,7 +1456,9 @@
       <c r="K3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="L3" s="2"/>
+      <c r="L3" s="2" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1346,6 +1494,9 @@
       <c r="K4" s="5" t="s">
         <v>51</v>
       </c>
+      <c r="L4" s="2" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1381,6 +1532,9 @@
       <c r="K5" s="5" t="s">
         <v>51</v>
       </c>
+      <c r="L5" s="2" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1415,6 +1569,9 @@
       </c>
       <c r="K6" s="5" t="s">
         <v>51</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -1434,8 +1591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4571448-FDFE-4F01-A516-0ABB06952D87}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,52 +1603,52 @@
     <col min="4" max="4" width="24.7109375" customWidth="1"/>
     <col min="5" max="5" width="75.7109375" style="8" customWidth="1"/>
     <col min="6" max="6" width="36" style="8" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" customWidth="1"/>
     <col min="8" max="8" width="40.140625" customWidth="1"/>
     <col min="9" max="9" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" customWidth="1"/>
     <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="15" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -1504,7 +1661,7 @@
       <c r="D2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="20" t="s">
         <v>110</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -1520,10 +1677,10 @@
         <v>66</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>67</v>
+        <v>238</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>67</v>
@@ -1567,11 +1724,11 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>58</v>
       </c>
       <c r="C4" s="12" t="s">
@@ -1583,29 +1740,29 @@
       <c r="E4" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>64</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -1621,29 +1778,29 @@
       <c r="E5" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="18" t="s">
         <v>64</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="L5" s="18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="17" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1659,29 +1816,29 @@
       <c r="E6" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="18" t="s">
         <v>64</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="K6" s="19" t="s">
+      <c r="K6" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="L6" s="18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>95</v>
       </c>
@@ -1770,11 +1927,11 @@
       <c r="D9" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="20" t="s">
         <v>119</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>64</v>
+        <v>239</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>120</v>
@@ -1799,7 +1956,7 @@
       <c r="D10" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="20" t="s">
         <v>125</v>
       </c>
       <c r="F10" s="7" t="s">
@@ -1828,7 +1985,7 @@
       <c r="D11" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="20" t="s">
         <v>128</v>
       </c>
       <c r="F11" s="7" t="s">
@@ -1851,7 +2008,7 @@
       <c r="D12" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="20" t="s">
         <v>130</v>
       </c>
       <c r="F12" s="7" t="s">
@@ -1874,7 +2031,7 @@
       <c r="D13" t="s">
         <v>124</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="20" t="s">
         <v>136</v>
       </c>
       <c r="F13" s="7" t="s">
@@ -1897,7 +2054,7 @@
       <c r="D14" t="s">
         <v>134</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="20" t="s">
         <v>137</v>
       </c>
       <c r="F14" s="7" t="s">
@@ -1920,7 +2077,7 @@
       <c r="D15" t="s">
         <v>135</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="20" t="s">
         <v>138</v>
       </c>
       <c r="F15" s="7" t="s">
@@ -1947,8 +2104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F819213-0935-4CCE-97BE-DCD2DE2E7E49}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView topLeftCell="E2" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1960,8 +2117,8 @@
     <col min="6" max="6" width="47" customWidth="1"/>
     <col min="7" max="7" width="22.85546875" customWidth="1"/>
     <col min="8" max="8" width="23" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="37.85546875" customWidth="1"/>
+    <col min="10" max="10" width="19" style="16" customWidth="1"/>
     <col min="11" max="11" width="13.140625" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" customWidth="1"/>
   </cols>
@@ -1970,46 +2127,46 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="20" t="s">
+      <c r="L2" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2030,11 +2187,24 @@
       <c r="G3" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="K3" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="2" t="s">
         <v>182</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2055,11 +2225,24 @@
       <c r="G4" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="2" t="s">
         <v>183</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -2080,11 +2263,24 @@
       <c r="G5" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="K5" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="2" t="s">
         <v>184</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -2105,11 +2301,24 @@
       <c r="G6" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="K6" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="2" t="s">
         <v>185</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2130,11 +2339,24 @@
       <c r="G7" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="H7" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="K7" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>186</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2155,11 +2377,24 @@
       <c r="G8" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="H8" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="I8" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="K8" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>187</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -2178,11 +2413,26 @@
         <v>200</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="K9" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>188</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2198,14 +2448,29 @@
         <v>177</v>
       </c>
       <c r="F10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="J10" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>189</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -2221,11 +2486,29 @@
         <v>178</v>
       </c>
       <c r="F11" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="I11" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="J11" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="K11" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>190</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -2241,11 +2524,29 @@
         <v>179</v>
       </c>
       <c r="F12" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+        <v>235</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="K12" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>191</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -2261,11 +2562,26 @@
         <v>180</v>
       </c>
       <c r="F13" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="K13" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>192</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -2281,11 +2597,50 @@
         <v>181</v>
       </c>
       <c r="F14" t="s">
-        <v>194</v>
+        <v>214</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="J14" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="K14" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AB0A0B2-B5F3-4A49-A089-B3D37B5BF24D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="255" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
TC for Product added
</commit_message>
<xml_diff>
--- a/Test-Cases.xlsx
+++ b/Test-Cases.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b69f171f4aec32e/Documents/GithubProjects/Manual-Testing-E-commerce-Amazon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="724" documentId="8_{815BE7B0-3C72-4824-8212-FAF9C84139DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54A1AFC5-327E-4AD0-AC23-6A33B094B1EA}"/>
+  <xr:revisionPtr revIDLastSave="995" documentId="8_{815BE7B0-3C72-4824-8212-FAF9C84139DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{586D4C42-FF9F-4D1B-A212-ECD2197B64E1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{6E1B6E8A-1244-4A63-966D-B4892D0CED0D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="3" xr2:uid="{6E1B6E8A-1244-4A63-966D-B4892D0CED0D}"/>
   </bookViews>
   <sheets>
     <sheet name="URL_Test_Cases" sheetId="1" r:id="rId1"/>
     <sheet name="User Registration_TestCases" sheetId="2" r:id="rId2"/>
     <sheet name="Login&amp;Logout_TestCases" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Product_Details_Test_Cases" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="332">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -861,6 +862,280 @@
   </si>
   <si>
     <t>Phone number Registered</t>
+  </si>
+  <si>
+    <t>User is on Product Details Page |</t>
+  </si>
+  <si>
+    <t>Product |</t>
+  </si>
+  <si>
+    <t>| | |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_PDP_01 </t>
+  </si>
+  <si>
+    <t>Product Details Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FR_PDP_01 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TS_PDP_01 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify product details are displayed correctly </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open a product details page
+2. Product
+</t>
+  </si>
+  <si>
+    <t>"Product name, brand,
+ and basic details are displayed "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is on Product Details Page </t>
+  </si>
+  <si>
+    <t>"Product name, brand,
+ and basic details are displayed  when opened product details page"</t>
+  </si>
+  <si>
+    <t>Verify product images are displayed |</t>
+  </si>
+  <si>
+    <t>1. View product images |</t>
+  </si>
+  <si>
+    <t>Product images are displayed correctly |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TC_PDP_02 | Product Details | </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR_PDP_02 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TS_PDP_02 </t>
+  </si>
+  <si>
+    <t>TC_PDP_02</t>
+  </si>
+  <si>
+    <t>TC_PDP_03</t>
+  </si>
+  <si>
+    <t>TC_PDP_04</t>
+  </si>
+  <si>
+    <t>TC_PDP_05</t>
+  </si>
+  <si>
+    <t>TC_PDP_06</t>
+  </si>
+  <si>
+    <t>TC_PDP_07</t>
+  </si>
+  <si>
+    <t>TC_PDP_08</t>
+  </si>
+  <si>
+    <t>TC_PDP_09</t>
+  </si>
+  <si>
+    <t>TC_PDP_10</t>
+  </si>
+  <si>
+    <t>TC_PDP_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Verify product images are displayed 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. View product images 
+Product </t>
+  </si>
+  <si>
+    <t>"Product images are
+ displayed correctly "</t>
+  </si>
+  <si>
+    <t>" Product images are
+ displayed correctly "</t>
+  </si>
+  <si>
+    <t>In-stock product</t>
+  </si>
+  <si>
+    <t>Verify product image zoom functionality</t>
+  </si>
+  <si>
+    <t>1.Hover or click on product image |
+Product</t>
+  </si>
+  <si>
+    <t>"Image zoom is dispalye
+correctly "</t>
+  </si>
+  <si>
+    <t>"Image zoomed and displayed
+correctly "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FR_PDP_03 </t>
+  </si>
+  <si>
+    <t>TS_PDP_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify product price is displayed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. View product price </t>
+  </si>
+  <si>
+    <t>"Correct product price 
+is displayed "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correct product price 
+is displayed </t>
+  </si>
+  <si>
+    <t>TS_PDP_04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify product availability status </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Check stock availability </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stock status (In stock / Out of stock) 
+is displayed </t>
+  </si>
+  <si>
+    <t>"Stock status (In stock / Out of stock) is displayed "</t>
+  </si>
+  <si>
+    <t>FR_PDP_04</t>
+  </si>
+  <si>
+    <t>FR_PDP_05</t>
+  </si>
+  <si>
+    <t>TS_PDP_05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user can select product quantity </t>
+  </si>
+  <si>
+    <t>\1. Select quantity from dropdown |
+Quantity</t>
+  </si>
+  <si>
+    <t>"Able to select quantity"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Quantity from dropdown should be selected" 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  NA</t>
+  </si>
+  <si>
+    <t>FR_PDP_06</t>
+  </si>
+  <si>
+    <t>TS_PDP_06</t>
+  </si>
+  <si>
+    <t>Quantity 1, 5</t>
+  </si>
+  <si>
+    <t>1. Observe Add to Cart button |</t>
+  </si>
+  <si>
+    <t>"Add to Cart button
+ is visible "</t>
+  </si>
+  <si>
+    <t>"Cart button visbile"</t>
+  </si>
+  <si>
+    <t>Verify Add to Cart button enabled for in-
+stock product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Add to Cart button is displayed </t>
+  </si>
+  <si>
+    <t>"Product is added 
+to cart successfully "</t>
+  </si>
+  <si>
+    <t>"Products can added to cart"</t>
+  </si>
+  <si>
+    <t>1. Click Add to Cart 
+Product</t>
+  </si>
+  <si>
+    <t>Verify Add to Cart is disabled for out-of-stock
+ product |</t>
+  </si>
+  <si>
+    <t>Out-stock product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Observe Add to Cart button |
+Product </t>
+  </si>
+  <si>
+    <t>"Add to Cart button is
+ disabled "</t>
+  </si>
+  <si>
+    <t>"Addcart button disbaled for out stock product"</t>
+  </si>
+  <si>
+    <t>TS_PDP_07</t>
+  </si>
+  <si>
+    <t>FR_PDP_07</t>
+  </si>
+  <si>
+    <t>Verify product description is displayed |</t>
+  </si>
+  <si>
+    <t>1. Scroll to description section |
+Product</t>
+  </si>
+  <si>
+    <t>"Product description 
+is displayed "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Product description is displayed" </t>
+  </si>
+  <si>
+    <t>Verify product specifications are displayed |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. View specifications section |
+Product </t>
+  </si>
+  <si>
+    <t>"Product specifications 
+are displayed |</t>
+  </si>
+  <si>
+    <t>"Product specifications are displayed "</t>
   </si>
 </sst>
 </file>
@@ -996,17 +1271,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1014,6 +1280,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1625,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4571448-FDFE-4F01-A516-0ABB06952D87}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="F11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,7 +1942,7 @@
       <c r="H1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="25" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="13" t="s">
@@ -1713,7 +1986,7 @@
       <c r="J2" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="24" t="s">
         <v>51</v>
       </c>
       <c r="L2" s="7" t="s">
@@ -1751,7 +2024,7 @@
       <c r="J3" t="s">
         <v>238</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="24" t="s">
         <v>51</v>
       </c>
       <c r="L3" t="s">
@@ -1789,7 +2062,7 @@
       <c r="J4" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="K4" s="27" t="s">
+      <c r="K4" s="24" t="s">
         <v>51</v>
       </c>
       <c r="L4" s="18" t="s">
@@ -1827,7 +2100,7 @@
       <c r="J5" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="K5" s="27" t="s">
+      <c r="K5" s="24" t="s">
         <v>51</v>
       </c>
       <c r="L5" s="18" t="s">
@@ -1865,7 +2138,7 @@
       <c r="J6" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="K6" s="27" t="s">
+      <c r="K6" s="24" t="s">
         <v>51</v>
       </c>
       <c r="L6" s="18" t="s">
@@ -1903,7 +2176,7 @@
       <c r="J7" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="K7" s="27" t="s">
+      <c r="K7" s="24" t="s">
         <v>51</v>
       </c>
       <c r="L7" s="7" t="s">
@@ -1941,7 +2214,7 @@
       <c r="J8" t="s">
         <v>243</v>
       </c>
-      <c r="K8" s="27" t="s">
+      <c r="K8" s="24" t="s">
         <v>51</v>
       </c>
       <c r="L8" t="s">
@@ -1979,7 +2252,7 @@
       <c r="J9" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="K9" s="27" t="s">
+      <c r="K9" s="24" t="s">
         <v>51</v>
       </c>
       <c r="L9" s="18" t="s">
@@ -2017,7 +2290,7 @@
       <c r="J10" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="K10" s="27" t="s">
+      <c r="K10" s="24" t="s">
         <v>51</v>
       </c>
       <c r="L10" s="18" t="s">
@@ -2052,7 +2325,7 @@
       <c r="J11" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="K11" s="27" t="s">
+      <c r="K11" s="24" t="s">
         <v>51</v>
       </c>
       <c r="L11" s="18" t="s">
@@ -2090,7 +2363,7 @@
       <c r="J12" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="K12" s="27" t="s">
+      <c r="K12" s="24" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2119,7 +2392,7 @@
       <c r="J13" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="K13" s="27" t="s">
+      <c r="K13" s="24" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2145,7 +2418,7 @@
       <c r="I14" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="K14" s="27" t="s">
+      <c r="K14" s="24" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2168,7 +2441,7 @@
       <c r="I15" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="K15" s="27" t="s">
+      <c r="K15" s="24" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2186,7 +2459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F819213-0935-4CCE-97BE-DCD2DE2E7E49}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView topLeftCell="E12" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -2278,7 +2551,7 @@
       <c r="J3" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="23" t="s">
         <v>51</v>
       </c>
       <c r="L3" t="s">
@@ -2310,13 +2583,13 @@
       <c r="H4" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="4" t="s">
         <v>219</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="23" t="s">
         <v>51</v>
       </c>
       <c r="L4" t="s">
@@ -2348,13 +2621,13 @@
       <c r="H5" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="4" t="s">
         <v>219</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="K5" s="26" t="s">
+      <c r="K5" s="23" t="s">
         <v>51</v>
       </c>
       <c r="L5" t="s">
@@ -2386,13 +2659,13 @@
       <c r="H6" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="4" t="s">
         <v>219</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="K6" s="26" t="s">
+      <c r="K6" s="23" t="s">
         <v>51</v>
       </c>
       <c r="L6" t="s">
@@ -2430,7 +2703,7 @@
       <c r="J7" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="K7" s="26" t="s">
+      <c r="K7" s="23" t="s">
         <v>51</v>
       </c>
       <c r="L7" t="s">
@@ -2462,13 +2735,13 @@
       <c r="H8" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="J8" s="25" t="s">
+      <c r="J8" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="K8" s="26" t="s">
+      <c r="K8" s="23" t="s">
         <v>51</v>
       </c>
       <c r="L8" t="s">
@@ -2500,13 +2773,13 @@
       <c r="H9" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="J9" s="25" t="s">
+      <c r="J9" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="23" t="s">
         <v>51</v>
       </c>
       <c r="L9" t="s">
@@ -2538,13 +2811,13 @@
       <c r="H10" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="J10" s="25" t="s">
+      <c r="J10" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="K10" s="26" t="s">
+      <c r="K10" s="23" t="s">
         <v>51</v>
       </c>
       <c r="L10" t="s">
@@ -2576,13 +2849,13 @@
       <c r="H11" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="J11" s="25" t="s">
+      <c r="J11" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="K11" s="26" t="s">
+      <c r="K11" s="23" t="s">
         <v>51</v>
       </c>
       <c r="L11" t="s">
@@ -2617,10 +2890,10 @@
       <c r="I12" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="J12" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="K12" s="26" t="s">
+      <c r="K12" s="23" t="s">
         <v>51</v>
       </c>
       <c r="L12" t="s">
@@ -2649,13 +2922,13 @@
       <c r="G13" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="22" t="s">
         <v>214</v>
       </c>
-      <c r="J13" s="25" t="s">
+      <c r="J13" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="K13" s="26" t="s">
+      <c r="K13" s="23" t="s">
         <v>51</v>
       </c>
       <c r="L13" t="s">
@@ -2687,13 +2960,13 @@
       <c r="H14" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="I14" s="23" t="s">
+      <c r="I14" s="22" t="s">
         <v>218</v>
       </c>
-      <c r="J14" s="25" t="s">
+      <c r="J14" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="K14" s="26" t="s">
+      <c r="K14" s="23" t="s">
         <v>51</v>
       </c>
       <c r="L14" t="s">
@@ -2708,17 +2981,537 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AB0A0B2-B5F3-4A49-A089-B3D37B5BF24D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="16" customWidth="1"/>
+    <col min="4" max="4" width="13" style="16" customWidth="1"/>
+    <col min="5" max="5" width="43.7109375" style="16" customWidth="1"/>
+    <col min="6" max="6" width="30" style="16" customWidth="1"/>
+    <col min="7" max="7" width="34.5703125" style="16" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="16" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="26" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="12"/>
+    <col min="12" max="12" width="9.140625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="16" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>266</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>267</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>298</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>293</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>294</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>295</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>313</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>309</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>324</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>322</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>328</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA327B7F-64E2-4FE3-AD7D-3A0C5D06EFA9}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
+      <c r="A1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>252</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
TC for order confrimation added
</commit_message>
<xml_diff>
--- a/Test-Cases.xlsx
+++ b/Test-Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b69f171f4aec32e/Documents/GithubProjects/Manual-Testing-E-commerce-Amazon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1773" documentId="8_{815BE7B0-3C72-4824-8212-FAF9C84139DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91F90952-3999-4FD6-9145-0B3D3B8500A2}"/>
+  <xr:revisionPtr revIDLastSave="1928" documentId="8_{815BE7B0-3C72-4824-8212-FAF9C84139DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD8404DD-AE93-43DE-83ED-E3CAEADF9CB1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="8" xr2:uid="{6E1B6E8A-1244-4A63-966D-B4892D0CED0D}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="629">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1972,9 +1972,6 @@
     <t>TC_OC_07</t>
   </si>
   <si>
-    <t>TC_OC_08</t>
-  </si>
-  <si>
     <t xml:space="preserve">Order Confirmation </t>
   </si>
   <si>
@@ -2006,6 +2003,141 @@
   <si>
     <t>"Order placed succesfully
  messgae displayed"</t>
+  </si>
+  <si>
+    <t>FR_OC_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  TS_OC_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order placed </t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>"Unique 
+order ID displayed "</t>
+  </si>
+  <si>
+    <t>"Unique order ID is
+generated"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify unique order
+ ID is generated </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify ordered product
+ details are displayed correctly </t>
+  </si>
+  <si>
+    <t>FR_OC_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  TS_OC_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. View order 
+confirmation page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. View order details </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ordered products </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Correct product, quantity, 
+and price displayed" </t>
+  </si>
+  <si>
+    <t>"All ordered details 
+displayed"</t>
+  </si>
+  <si>
+    <t>Verify payment status 
+is displayed correctly</t>
+  </si>
+  <si>
+    <t>FR_OC_04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  TS_OC_04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. View payment status 
+</t>
+  </si>
+  <si>
+    <t>"Payment
+ status shown as Successful"</t>
+  </si>
+  <si>
+    <t>FR_OC_05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  TS_OC_05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify order confirmation 
+message is displayed </t>
+  </si>
+  <si>
+    <t>Order placed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Observe confirmation
+ message </t>
+  </si>
+  <si>
+    <t>"Order placed 
+successfully message displayed "</t>
+  </si>
+  <si>
+    <t>FR_OC_06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  TS_OC_06</t>
+  </si>
+  <si>
+    <t>User logged in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Navigate to My Orders </t>
+  </si>
+  <si>
+    <t>"Order appears 
+in My Orders list "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify confirmation 
+email/SMS is sent </t>
+  </si>
+  <si>
+    <t>FR_OC_07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  TS_OC_07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify placed order is
+ visible in My Orders section </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Check registered email/SMS </t>
+  </si>
+  <si>
+    <t>Email/Sms</t>
+  </si>
+  <si>
+    <t>"Order confirmation 
+notification received "</t>
+  </si>
+  <si>
+    <t>"Order 
+confirmation notification received "</t>
   </si>
 </sst>
 </file>
@@ -2076,7 +2208,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2151,7 +2283,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2166,6 +2297,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3877,7 +4017,7 @@
     <col min="7" max="7" width="34.5703125" style="16" customWidth="1"/>
     <col min="8" max="8" width="15.5703125" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" style="16" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="26" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
     <col min="11" max="11" width="9.140625" style="12"/>
     <col min="12" max="12" width="9.140625" style="16"/>
   </cols>
@@ -3898,7 +4038,7 @@
       <c r="E1" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="27" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="25" t="s">
@@ -3913,7 +4053,7 @@
       <c r="J1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="26" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="25" t="s">
@@ -3951,7 +4091,7 @@
       <c r="J2" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="28" t="s">
         <v>51</v>
       </c>
       <c r="L2" s="16" t="s">
@@ -3989,7 +4129,7 @@
       <c r="J3" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="28" t="s">
         <v>51</v>
       </c>
       <c r="L3" s="16" t="s">
@@ -4027,7 +4167,7 @@
       <c r="J4" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="K4" s="29" t="s">
+      <c r="K4" s="28" t="s">
         <v>51</v>
       </c>
       <c r="L4" s="16" t="s">
@@ -4065,7 +4205,7 @@
       <c r="J5" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="K5" s="29" t="s">
+      <c r="K5" s="28" t="s">
         <v>51</v>
       </c>
       <c r="L5" s="16" t="s">
@@ -4103,7 +4243,7 @@
       <c r="J6" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="K6" s="29" t="s">
+      <c r="K6" s="28" t="s">
         <v>51</v>
       </c>
       <c r="L6" s="16" t="s">
@@ -4141,7 +4281,7 @@
       <c r="J7" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="K7" s="29" t="s">
+      <c r="K7" s="28" t="s">
         <v>51</v>
       </c>
       <c r="L7" s="16" t="s">
@@ -4179,7 +4319,7 @@
       <c r="J8" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="K8" s="29" t="s">
+      <c r="K8" s="28" t="s">
         <v>51</v>
       </c>
       <c r="L8" s="16" t="s">
@@ -4217,7 +4357,7 @@
       <c r="J9" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="K9" s="29" t="s">
+      <c r="K9" s="28" t="s">
         <v>51</v>
       </c>
       <c r="L9" s="16" t="s">
@@ -4255,7 +4395,7 @@
       <c r="J10" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="K10" s="29" t="s">
+      <c r="K10" s="28" t="s">
         <v>51</v>
       </c>
       <c r="L10" s="16" t="s">
@@ -4293,7 +4433,7 @@
       <c r="J11" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="K11" s="29" t="s">
+      <c r="K11" s="28" t="s">
         <v>51</v>
       </c>
       <c r="L11" s="16" t="s">
@@ -4331,7 +4471,7 @@
       <c r="J12" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="K12" s="29" t="s">
+      <c r="K12" s="28" t="s">
         <v>51</v>
       </c>
       <c r="L12" s="16" t="s">
@@ -4370,7 +4510,7 @@
       <c r="A1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="25" t="s">
@@ -4382,7 +4522,7 @@
       <c r="E1" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="27" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="25" t="s">
@@ -4404,29 +4544,29 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="26" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>325</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" t="s">
         <v>326</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" t="s">
         <v>327</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" t="s">
         <v>328</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" t="s">
         <v>335</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" t="s">
         <v>336</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" t="s">
         <v>338</v>
       </c>
       <c r="I2" s="2" t="s">
@@ -4449,22 +4589,22 @@
       <c r="B3" t="s">
         <v>326</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" t="s">
         <v>341</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" t="s">
         <v>345</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" t="s">
         <v>336</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" t="s">
         <v>338</v>
       </c>
       <c r="I3" s="4" t="s">
@@ -4487,16 +4627,16 @@
       <c r="B4" t="s">
         <v>326</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" t="s">
         <v>342</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" t="s">
         <v>346</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" t="s">
         <v>353</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -4525,16 +4665,16 @@
       <c r="B5" t="s">
         <v>326</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" t="s">
         <v>342</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" t="s">
         <v>346</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" t="s">
         <v>353</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -4563,16 +4703,16 @@
       <c r="B6" t="s">
         <v>326</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" t="s">
         <v>342</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" t="s">
         <v>346</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>371</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" t="s">
         <v>372</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -4601,10 +4741,10 @@
       <c r="B7" t="s">
         <v>326</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" t="s">
         <v>343</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" t="s">
         <v>347</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -4639,16 +4779,16 @@
       <c r="B8" t="s">
         <v>326</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" t="s">
         <v>344</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" t="s">
         <v>348</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>368</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" t="s">
         <v>336</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -4702,7 +4842,7 @@
       <c r="A1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="25" t="s">
@@ -4714,7 +4854,7 @@
       <c r="E1" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="27" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="25" t="s">
@@ -5058,7 +5198,7 @@
       <c r="A1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="25" t="s">
@@ -5070,7 +5210,7 @@
       <c r="E1" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="27" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="25" t="s">
@@ -5155,7 +5295,7 @@
       <c r="J3" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="K3" s="31" t="s">
+      <c r="K3" s="30" t="s">
         <v>51</v>
       </c>
       <c r="L3" s="16" t="s">
@@ -5190,7 +5330,7 @@
       <c r="J4" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="K4" s="31" t="s">
+      <c r="K4" s="30" t="s">
         <v>51</v>
       </c>
       <c r="L4" s="16" t="s">
@@ -5446,7 +5586,7 @@
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="26" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
     <col min="7" max="7" width="23.140625" customWidth="1"/>
     <col min="8" max="8" width="19.5703125" customWidth="1"/>
     <col min="9" max="9" width="25.140625" style="16" customWidth="1"/>
@@ -5457,7 +5597,7 @@
       <c r="A1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="25" t="s">
@@ -5522,7 +5662,7 @@
       <c r="J2" s="2" t="s">
         <v>526</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="30" t="s">
         <v>51</v>
       </c>
       <c r="L2" s="16" t="s">
@@ -5560,7 +5700,7 @@
       <c r="J3" s="2" t="s">
         <v>534</v>
       </c>
-      <c r="K3" s="31" t="s">
+      <c r="K3" s="30" t="s">
         <v>51</v>
       </c>
       <c r="L3" s="16" t="s">
@@ -5598,7 +5738,7 @@
       <c r="J4" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="K4" s="31" t="s">
+      <c r="K4" s="30" t="s">
         <v>51</v>
       </c>
       <c r="L4" s="16" t="s">
@@ -5636,14 +5776,14 @@
       <c r="J5" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="K5" s="31" t="s">
+      <c r="K5" s="30" t="s">
         <v>51</v>
       </c>
       <c r="L5" s="16" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>509</v>
       </c>
@@ -5674,7 +5814,7 @@
       <c r="J6" s="4" t="s">
         <v>550</v>
       </c>
-      <c r="K6" s="31" t="s">
+      <c r="K6" s="30" t="s">
         <v>51</v>
       </c>
       <c r="L6" s="16" t="s">
@@ -5712,14 +5852,14 @@
       <c r="J7" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="K7" s="31" t="s">
+      <c r="K7" s="30" t="s">
         <v>51</v>
       </c>
       <c r="L7" s="16" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="16" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>511</v>
       </c>
@@ -5750,7 +5890,7 @@
       <c r="J8" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="K8" s="31" t="s">
+      <c r="K8" s="30" t="s">
         <v>51</v>
       </c>
       <c r="L8" s="16" t="s">
@@ -5785,7 +5925,7 @@
       <c r="J9" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="K9" s="31" t="s">
+      <c r="K9" s="30" t="s">
         <v>51</v>
       </c>
       <c r="L9" s="16" t="s">
@@ -5823,7 +5963,7 @@
       <c r="J10" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="K10" s="31" t="s">
+      <c r="K10" s="30" t="s">
         <v>51</v>
       </c>
       <c r="L10" s="16" t="s">
@@ -5841,31 +5981,33 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8983707B-2900-4232-B9A4-6CEF831CF204}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="16" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
     <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="17" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="14" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" style="14" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="14"/>
+    <col min="12" max="12" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="25" t="s">
@@ -5874,123 +6016,295 @@
       <c r="D1" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="14" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>574</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>581</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>582</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="D2" s="14" t="s">
         <v>583</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="29" t="s">
         <v>584</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="F2" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="G2" s="7" t="s">
         <v>586</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="H2" s="29" t="s">
         <v>587</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="I2" s="29" t="s">
         <v>588</v>
       </c>
-      <c r="I2" s="30" t="s">
+      <c r="J2" s="29" t="s">
         <v>589</v>
       </c>
-      <c r="J2" s="30" t="s">
+      <c r="K2" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>581</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>590</v>
       </c>
-      <c r="K2" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>575</v>
-      </c>
-      <c r="B3" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D3" s="14" t="s">
+        <v>591</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>596</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>593</v>
+      </c>
+      <c r="I3" s="29" t="s">
+        <v>594</v>
+      </c>
+      <c r="J3" s="29" t="s">
+        <v>595</v>
+      </c>
+      <c r="K3" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>576</v>
       </c>
-      <c r="B4" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" s="16" t="s">
+        <v>581</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>598</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>599</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>597</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>601</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>602</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>603</v>
+      </c>
+      <c r="J4" s="29" t="s">
+        <v>604</v>
+      </c>
+      <c r="K4" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="32" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>577</v>
       </c>
-      <c r="B5" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" s="14" t="s">
+        <v>581</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>606</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>607</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>605</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>608</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>514</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>609</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>609</v>
+      </c>
+      <c r="K5" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" s="32" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>578</v>
       </c>
-      <c r="B6" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B6" s="16" t="s">
+        <v>581</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>610</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>611</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>612</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>613</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>593</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>615</v>
+      </c>
+      <c r="J6" s="29" t="s">
+        <v>615</v>
+      </c>
+      <c r="K6" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>579</v>
       </c>
-      <c r="B7" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B7" s="16" t="s">
+        <v>581</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>616</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>617</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>624</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>618</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>619</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>593</v>
+      </c>
+      <c r="I7" s="29" t="s">
+        <v>620</v>
+      </c>
+      <c r="J7" s="29" t="s">
+        <v>620</v>
+      </c>
+      <c r="K7" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>580</v>
       </c>
-      <c r="B8" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B8" s="16" t="s">
         <v>581</v>
       </c>
-      <c r="B9" t="s">
-        <v>582</v>
+      <c r="C8" s="14" t="s">
+        <v>622</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>621</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>613</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>625</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>626</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>627</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>628</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>